<commit_message>
Updated Ruby Examples to use common data folder
</commit_message>
<xml_diff>
--- a/Data/Sample_Book1.xlsx
+++ b/Data/Sample_Book1.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\www\autogen\examples\Cells\src\Data\Input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="13275" windowHeight="8955" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,14 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -84,15 +74,10 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -137,46 +122,121 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma" xfId="4"/>
-    <cellStyle name="Comma [0]" xfId="5"/>
-    <cellStyle name="Currency" xfId="2"/>
-    <cellStyle name="Currency [0]" xfId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1"/>
+    <cellStyle name="Normal" xfId="0"/>
+    <cellStyle name="Percent" xfId="15"/>
+    <cellStyle name="Currency" xfId="16"/>
+    <cellStyle name="Currency [0]" xfId="17"/>
+    <cellStyle name="Comma" xfId="18"/>
+    <cellStyle name="Comma [0]" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -435,254 +495,256 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="20.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="12.75">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="12.75">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="5" spans="1:8" ht="12.75">
+      <c r="A5" s="5">
         <v>12</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>23</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>33</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>66</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>11</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>87</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>99</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="6" spans="1:8" ht="12.75">
+      <c r="A6" s="5">
         <v>23</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>22</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>33</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>77</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>31</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>22</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>45</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+    <row r="7" spans="1:8" ht="12.75">
+      <c r="A7" s="5">
         <v>34</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>12</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>23</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>22</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>34</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>11</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+    <row r="8" spans="1:8" ht="12.75">
+      <c r="A8" s="5">
         <v>45</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>43</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>54</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>88</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>36</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>45</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>45</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+    <row r="9" spans="1:8" ht="12.75">
+      <c r="A9" s="5">
         <v>65</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>65</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>65</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>65</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>13</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>65</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>9</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+    <row r="10" spans="1:8" ht="12.75">
+      <c r="A10" s="5">
         <v>34</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>22</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>27</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>22</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>32</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>23</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>23</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <f t="shared" ref="A11:H11" si="0">SUM(A5:A10)</f>
+    <row r="11" spans="1:8" ht="12.75">
+      <c r="A11" s="5">
+        <f t="shared" si="0" ref="A11:H11">SUM(A5:A10)</f>
         <v>213</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>341</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>276</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>232</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
         <v>205</v>
       </c>
@@ -692,7 +754,7 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>